<commit_message>
Adding few more testcases & adding the description for Pagefactory
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,13 +41,13 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Dee689</t>
-  </si>
-  <si>
-    <t>veer59</t>
-  </si>
-  <si>
-    <t>Y!7e3mV#</t>
+    <t>Deem753</t>
+  </si>
+  <si>
+    <t>veer33</t>
+  </si>
+  <si>
+    <t>aP$32r%K</t>
   </si>
   <si>
     <t>MR</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23070335</v>
+        <v>23070701</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added iProctor Regression TC'S
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Deem618</t>
-  </si>
-  <si>
-    <t>rahulrcb728</t>
-  </si>
-  <si>
-    <t>ak!D3#4B</t>
-  </si>
-  <si>
-    <t>MR</t>
-  </si>
-  <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Ka</t>
+    <t>Dee165</t>
+  </si>
+  <si>
+    <t>jadeja94</t>
+  </si>
+  <si>
+    <t>tY73%&amp;Sc</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>Jadeja</t>
+  </si>
+  <si>
+    <t>Bhaiu</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23070734</v>
+        <v>23071031</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added regression test cases for iProctor
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Deem618</t>
-  </si>
-  <si>
-    <t>rahulrcb728</t>
-  </si>
-  <si>
-    <t>ak!D3#4B</t>
+    <t>test825</t>
+  </si>
+  <si>
+    <t>narendra91</t>
+  </si>
+  <si>
+    <t>s5U%8$fB</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Ka</t>
+    <t>Narendra</t>
+  </si>
+  <si>
+    <t>Modi</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23070734</v>
+        <v>23071033</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added iProctor Regression TC-27,28 and 32
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,13 +41,13 @@
     <t>Role</t>
   </si>
   <si>
-    <t>test825</t>
-  </si>
-  <si>
-    <t>narendra91</t>
-  </si>
-  <si>
-    <t>s5U%8$fB</t>
+    <t>test114</t>
+  </si>
+  <si>
+    <t>narendra62</t>
+  </si>
+  <si>
+    <t>T3#%gA2b</t>
   </si>
   <si>
     <t>MR</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23071033</v>
+        <v>23071147</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding regression test cases
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,13 +41,13 @@
     <t>Role</t>
   </si>
   <si>
-    <t>test872</t>
-  </si>
-  <si>
-    <t>narendra57</t>
-  </si>
-  <si>
-    <t>P&amp;Kb7t2#</t>
+    <t>test201</t>
+  </si>
+  <si>
+    <t>narendra658</t>
+  </si>
+  <si>
+    <t>S#w3Kk7%</t>
   </si>
   <si>
     <t>MR</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23071150</v>
+        <v>23071223</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added iProctor Regression TC-33,46,93 and 94
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,13 +41,13 @@
     <t>Role</t>
   </si>
   <si>
-    <t>test872</t>
-  </si>
-  <si>
-    <t>narendra57</t>
-  </si>
-  <si>
-    <t>P&amp;Kb7t2#</t>
+    <t>test461</t>
+  </si>
+  <si>
+    <t>narendra695</t>
+  </si>
+  <si>
+    <t>m4s$!W5E</t>
   </si>
   <si>
     <t>MR</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23071150</v>
+        <v>23071214</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added iProctor Reg TC-33,46,93 and 94
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,13 +41,13 @@
     <t>Role</t>
   </si>
   <si>
-    <t>test461</t>
-  </si>
-  <si>
-    <t>narendra695</t>
-  </si>
-  <si>
-    <t>m4s$!W5E</t>
+    <t>test201</t>
+  </si>
+  <si>
+    <t>narendra658</t>
+  </si>
+  <si>
+    <t>S#w3Kk7%</t>
   </si>
   <si>
     <t>MR</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23071214</v>
+        <v>23071223</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added iProctor Reg TC-121,122 and 123
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,13 +41,13 @@
     <t>Role</t>
   </si>
   <si>
-    <t>test201</t>
-  </si>
-  <si>
-    <t>narendra658</t>
-  </si>
-  <si>
-    <t>S#w3Kk7%</t>
+    <t>test993</t>
+  </si>
+  <si>
+    <t>narendra676</t>
+  </si>
+  <si>
+    <t>Y$k2&amp;9aE</t>
   </si>
   <si>
     <t>MR</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23071223</v>
+        <v>23071337</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added New Tc's and 1 modified Tc
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,13 +41,13 @@
     <t>Role</t>
   </si>
   <si>
-    <t>test201</t>
-  </si>
-  <si>
-    <t>narendra658</t>
-  </si>
-  <si>
-    <t>S#w3Kk7%</t>
+    <t>test985</t>
+  </si>
+  <si>
+    <t>narendra6643</t>
+  </si>
+  <si>
+    <t>s%7#5hDB</t>
   </si>
   <si>
     <t>MR</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23071223</v>
+        <v>23071334</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added iProctor Reg TC-124 and 125
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>test875</t>
-  </si>
-  <si>
-    <t>narendra694</t>
-  </si>
-  <si>
-    <t>Ch$6n5#J</t>
+    <t>testsand316</t>
+  </si>
+  <si>
+    <t>igs52</t>
+  </si>
+  <si>
+    <t>Ek6!J$z4</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>Narendra</t>
-  </si>
-  <si>
-    <t>Modi</t>
+    <t>IGS</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23071343</v>
+        <v>23071457</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added iProctor Reg TC-126,127,128,129,143 and 144
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>testsand316</t>
-  </si>
-  <si>
-    <t>igs52</t>
-  </si>
-  <si>
-    <t>Ek6!J$z4</t>
+    <t>XTzVQ360</t>
+  </si>
+  <si>
+    <t>gglvyxp82</t>
+  </si>
+  <si>
+    <t>vf8#4$EV</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>IGS</t>
-  </si>
-  <si>
-    <t>India</t>
+    <t>vbGGAtLy</t>
+  </si>
+  <si>
+    <t>OHsZ</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23071457</v>
+        <v>23071736</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding iExam and iProctor TC's
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,13 +41,13 @@
     <t>Role</t>
   </si>
   <si>
-    <t>test875</t>
-  </si>
-  <si>
-    <t>narendra694</t>
-  </si>
-  <si>
-    <t>Ch$6n5#J</t>
+    <t>test353</t>
+  </si>
+  <si>
+    <t>narendra681</t>
+  </si>
+  <si>
+    <t>w59!TP#v</t>
   </si>
   <si>
     <t>MR</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23071343</v>
+        <v>23071746</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added iProctor Reg TC-36,88,89,90,92 and 120
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>XTzVQ360</t>
-  </si>
-  <si>
-    <t>gglvyxp82</t>
-  </si>
-  <si>
-    <t>vf8#4$EV</t>
+    <t>OOkLX161</t>
+  </si>
+  <si>
+    <t>urfnboj78</t>
+  </si>
+  <si>
+    <t>KN&amp;8w7j%</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>vbGGAtLy</t>
-  </si>
-  <si>
-    <t>OHsZ</t>
+    <t>RXpSxSmD</t>
+  </si>
+  <si>
+    <t>reGn</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23071736</v>
+        <v>23071823</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added more regression testcases and updated changes
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>XTzVQ360</t>
-  </si>
-  <si>
-    <t>gglvyxp82</t>
-  </si>
-  <si>
-    <t>vf8#4$EV</t>
+    <t>ocYZK178</t>
+  </si>
+  <si>
+    <t>kowgmyl87</t>
+  </si>
+  <si>
+    <t>ZU%3yq6$</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>vbGGAtLy</t>
-  </si>
-  <si>
-    <t>OHsZ</t>
+    <t>JDSAlTPD</t>
+  </si>
+  <si>
+    <t>eHch</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23071736</v>
+        <v>23071818</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
resolving merge conflicts for Arish
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>CGdcG599</t>
-  </si>
-  <si>
-    <t>pxpieqd10</t>
-  </si>
-  <si>
-    <t>u&amp;6bK#P3</t>
+    <t>OOkLX161</t>
+  </si>
+  <si>
+    <t>urfnboj78</t>
+  </si>
+  <si>
+    <t>KN&amp;8w7j%</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>CAKyNogI</t>
-  </si>
-  <si>
-    <t>PHYM</t>
+    <t>RXpSxSmD</t>
+  </si>
+  <si>
+    <t>reGn</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23071822</v>
+        <v>23071823</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
modified testcases and added search exam for the TC's
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>OOkLX161</t>
-  </si>
-  <si>
-    <t>urfnboj78</t>
-  </si>
-  <si>
-    <t>KN&amp;8w7j%</t>
+    <t>MXato821</t>
+  </si>
+  <si>
+    <t>hjuzqjd22</t>
+  </si>
+  <si>
+    <t>sH#c5%2D</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>RXpSxSmD</t>
-  </si>
-  <si>
-    <t>reGn</t>
+    <t>ppxFBVUI</t>
+  </si>
+  <si>
+    <t>ZlSl</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23071823</v>
+        <v>23071960</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added iProctor Reg TC-83
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>OOkLX161</t>
-  </si>
-  <si>
-    <t>urfnboj78</t>
-  </si>
-  <si>
-    <t>KN&amp;8w7j%</t>
+    <t>wYCsK239</t>
+  </si>
+  <si>
+    <t>yhzsxcy35</t>
+  </si>
+  <si>
+    <t>k8$Qt2Z#</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>RXpSxSmD</t>
-  </si>
-  <si>
-    <t>reGn</t>
+    <t>czuFDRuU</t>
+  </si>
+  <si>
+    <t>cafp</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23071823</v>
+        <v>23071982</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added 6 Test Scripts
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>OOkLX161</t>
-  </si>
-  <si>
-    <t>urfnboj78</t>
-  </si>
-  <si>
-    <t>KN&amp;8w7j%</t>
+    <t>MdKbD525</t>
+  </si>
+  <si>
+    <t>vifsyvt95</t>
+  </si>
+  <si>
+    <t>QF&amp;8re!9</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>RXpSxSmD</t>
-  </si>
-  <si>
-    <t>reGn</t>
+    <t>XWzRTWDw</t>
+  </si>
+  <si>
+    <t>EWtC</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23071823</v>
+        <v>23071985</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
optimising the code for page factory
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>MXato821</t>
-  </si>
-  <si>
-    <t>hjuzqjd22</t>
-  </si>
-  <si>
-    <t>sH#c5%2D</t>
+    <t>sdtSm161</t>
+  </si>
+  <si>
+    <t>dfcmoru15</t>
+  </si>
+  <si>
+    <t>gWq42M#!</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>ppxFBVUI</t>
-  </si>
-  <si>
-    <t>ZlSl</t>
+    <t>RNODCaqD</t>
+  </si>
+  <si>
+    <t>avVL</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23071960</v>
+        <v>23072050</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding changes to inv page factory
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>sdtSm161</t>
-  </si>
-  <si>
-    <t>dfcmoru15</t>
-  </si>
-  <si>
-    <t>gWq42M#!</t>
+    <t>DUuJL107</t>
+  </si>
+  <si>
+    <t>uzqkqgb14</t>
+  </si>
+  <si>
+    <t>Q4#7$aSf</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>RNODCaqD</t>
-  </si>
-  <si>
-    <t>avVL</t>
+    <t>ELlZtVht</t>
+  </si>
+  <si>
+    <t>FKqC</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23072050</v>
+        <v>23072139</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Modified test cases and pages in page factory
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>sdtSm161</t>
-  </si>
-  <si>
-    <t>dfcmoru15</t>
-  </si>
-  <si>
-    <t>gWq42M#!</t>
+    <t>xJafy493</t>
+  </si>
+  <si>
+    <t>neowgrv38</t>
+  </si>
+  <si>
+    <t>t5#8Pn$Q</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>RNODCaqD</t>
-  </si>
-  <si>
-    <t>avVL</t>
+    <t>nbmsDSUi</t>
+  </si>
+  <si>
+    <t>YIOp</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23072050</v>
+        <v>23072455</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added Modified iProctor TC's
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>MhMUC745</t>
-  </si>
-  <si>
-    <t>dxzypke86</t>
-  </si>
-  <si>
-    <t>CeA27$d!</t>
+    <t>csAUq754</t>
+  </si>
+  <si>
+    <t>jtyhqyk59</t>
+  </si>
+  <si>
+    <t>r38!vMV$</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>rMTQpKZe</t>
-  </si>
-  <si>
-    <t>jHJq</t>
+    <t>QJgaITVt</t>
+  </si>
+  <si>
+    <t>tLjA</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23072501</v>
+        <v>23072557</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding changes to 1TC and making changes to Page Factory
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>MhMUC745</t>
-  </si>
-  <si>
-    <t>dxzypke86</t>
-  </si>
-  <si>
-    <t>CeA27$d!</t>
+    <t>MECit547</t>
+  </si>
+  <si>
+    <t>sffmqsl59</t>
+  </si>
+  <si>
+    <t>Nc6q!T$4</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>rMTQpKZe</t>
-  </si>
-  <si>
-    <t>jHJq</t>
+    <t>MajCmAme</t>
+  </si>
+  <si>
+    <t>yZFB</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23072501</v>
+        <v>23072604</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding Optimized TC's 3
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>csAUq754</t>
-  </si>
-  <si>
-    <t>jtyhqyk59</t>
-  </si>
-  <si>
-    <t>r38!vMV$</t>
+    <t>YGptT120</t>
+  </si>
+  <si>
+    <t>yvzdqcq33</t>
+  </si>
+  <si>
+    <t>Hx4&amp;3n#W</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>QJgaITVt</t>
-  </si>
-  <si>
-    <t>tLjA</t>
+    <t>hhvrnRtD</t>
+  </si>
+  <si>
+    <t>MKqD</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23072557</v>
+        <v>23072636</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added Modified Reg iProctor TC's
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>YGptT120</t>
-  </si>
-  <si>
-    <t>yvzdqcq33</t>
-  </si>
-  <si>
-    <t>Hx4&amp;3n#W</t>
+    <t>YBuqd553</t>
+  </si>
+  <si>
+    <t>peglstf18</t>
+  </si>
+  <si>
+    <t>Bv%&amp;J93u</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>hhvrnRtD</t>
-  </si>
-  <si>
-    <t>MKqD</t>
+    <t>JoyaOucZ</t>
+  </si>
+  <si>
+    <t>rCEY</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23072636</v>
+        <v>23072720</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding changes to iProctor Smoke and updating some regression tests
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>YGptT120</t>
-  </si>
-  <si>
-    <t>yvzdqcq33</t>
-  </si>
-  <si>
-    <t>Hx4&amp;3n#W</t>
+    <t>QzBON561</t>
+  </si>
+  <si>
+    <t>gtbcicg49</t>
+  </si>
+  <si>
+    <t>Rf5&amp;4Fp%</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>hhvrnRtD</t>
-  </si>
-  <si>
-    <t>MKqD</t>
+    <t>EdwytpvL</t>
+  </si>
+  <si>
+    <t>EIzt</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23072636</v>
+        <v>23072734</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
adding date and min changes
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>YBuqd553</t>
-  </si>
-  <si>
-    <t>peglstf18</t>
-  </si>
-  <si>
-    <t>Bv%&amp;J93u</t>
+    <t>nvTmX183</t>
+  </si>
+  <si>
+    <t>jwwcmjx39</t>
+  </si>
+  <si>
+    <t>kAX3m#9&amp;</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>JoyaOucZ</t>
-  </si>
-  <si>
-    <t>rCEY</t>
+    <t>JjmTLqRU</t>
+  </si>
+  <si>
+    <t>xaTn</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23072720</v>
+        <v>23073105</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
adding date changes to page factory
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>nvTmX183</t>
-  </si>
-  <si>
-    <t>jwwcmjx39</t>
-  </si>
-  <si>
-    <t>kAX3m#9&amp;</t>
+    <t>AgGbg661</t>
+  </si>
+  <si>
+    <t>gvxdihi52</t>
+  </si>
+  <si>
+    <t>Qf#8$9mA</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>JjmTLqRU</t>
-  </si>
-  <si>
-    <t>xaTn</t>
+    <t>AAKFrBgj</t>
+  </si>
+  <si>
+    <t>idAs</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23073105</v>
+        <v>23073124</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added Modified Reg iExam TC's
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>AgGbg661</t>
-  </si>
-  <si>
-    <t>gvxdihi52</t>
-  </si>
-  <si>
-    <t>Qf#8$9mA</t>
+    <t>degHh927</t>
+  </si>
+  <si>
+    <t>rchbrlj12</t>
+  </si>
+  <si>
+    <t>h%8eB5!N</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>AAKFrBgj</t>
-  </si>
-  <si>
-    <t>idAs</t>
+    <t>BDQEAMiI</t>
+  </si>
+  <si>
+    <t>sYkg</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23073124</v>
+        <v>23080135</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding Logout for all the smoke suite
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>degHh927</t>
-  </si>
-  <si>
-    <t>rchbrlj12</t>
-  </si>
-  <si>
-    <t>h%8eB5!N</t>
+    <t>CLfwZ777</t>
+  </si>
+  <si>
+    <t>kaqhund46</t>
+  </si>
+  <si>
+    <t>wY8$X%2n</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>BDQEAMiI</t>
-  </si>
-  <si>
-    <t>sYkg</t>
+    <t>SIJjvdpw</t>
+  </si>
+  <si>
+    <t>YBKM</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23080135</v>
+        <v>23080256</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding testcases of p2,p3
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>rpZLs656</t>
-  </si>
-  <si>
-    <t>hkmkdsh13</t>
-  </si>
-  <si>
-    <t>Dma5W7%!</t>
+    <t>nvOfx812</t>
+  </si>
+  <si>
+    <t>gkicyka73</t>
+  </si>
+  <si>
+    <t>Z&amp;#We6f3</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>NtQlFPxc</t>
-  </si>
-  <si>
-    <t>WQWc</t>
+    <t>eToTjsaw</t>
+  </si>
+  <si>
+    <t>wxeQ</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23080424</v>
+        <v>23080714</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added Modified Reg iExam P2,P3 TC's
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>rpZLs656</t>
-  </si>
-  <si>
-    <t>hkmkdsh13</t>
-  </si>
-  <si>
-    <t>Dma5W7%!</t>
+    <t>TlcTL154</t>
+  </si>
+  <si>
+    <t>itfhqke80</t>
+  </si>
+  <si>
+    <t>q8&amp;eG3#E</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>NtQlFPxc</t>
-  </si>
-  <si>
-    <t>WQWc</t>
+    <t>AgynuRYv</t>
+  </si>
+  <si>
+    <t>XvtW</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23080424</v>
+        <v>23080719</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding 4 TC's of P2,P3
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>QfVkf357</t>
-  </si>
-  <si>
-    <t>xeoloyz63</t>
-  </si>
-  <si>
-    <t>Ps4u$6%U</t>
+    <t>FCLXw697</t>
+  </si>
+  <si>
+    <t>hwgktnx59</t>
+  </si>
+  <si>
+    <t>h8!7#QBp</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>kiWrVdoY</t>
-  </si>
-  <si>
-    <t>FCgB</t>
+    <t>RpFFQEZI</t>
+  </si>
+  <si>
+    <t>Feuq</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23080917</v>
+        <v>23081037</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added Modified Reg iExam and iProctor P2,P3 TC's
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>QfVkf357</t>
-  </si>
-  <si>
-    <t>xeoloyz63</t>
-  </si>
-  <si>
-    <t>Ps4u$6%U</t>
+    <t>gATGO674</t>
+  </si>
+  <si>
+    <t>ubzzrnn59</t>
+  </si>
+  <si>
+    <t>rj82JD&amp;$</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>kiWrVdoY</t>
-  </si>
-  <si>
-    <t>FCgB</t>
+    <t>gknOSSlg</t>
+  </si>
+  <si>
+    <t>LCJs</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23080917</v>
+        <v>23081034</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding TC's of P2,P3
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>FCLXw697</t>
-  </si>
-  <si>
-    <t>hwgktnx59</t>
-  </si>
-  <si>
-    <t>h8!7#QBp</t>
+    <t>fSgDQ134</t>
+  </si>
+  <si>
+    <t>rkowlyw64</t>
+  </si>
+  <si>
+    <t>dMvH$2&amp;6</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>RpFFQEZI</t>
-  </si>
-  <si>
-    <t>Feuq</t>
+    <t>DAeTNpEK</t>
+  </si>
+  <si>
+    <t>Rmvc</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23081037</v>
+        <v>23081404</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added Modified Reg iProctor P2,P3 TC's
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>FCLXw697</t>
-  </si>
-  <si>
-    <t>hwgktnx59</t>
-  </si>
-  <si>
-    <t>h8!7#QBp</t>
+    <t>xdCzd476</t>
+  </si>
+  <si>
+    <t>dflgtzp77</t>
+  </si>
+  <si>
+    <t>j#8SkF$6</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>RpFFQEZI</t>
-  </si>
-  <si>
-    <t>Feuq</t>
+    <t>CKywQwIb</t>
+  </si>
+  <si>
+    <t>IKYx</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23081037</v>
+        <v>23081409</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding changes to date & time and tests in P2,P3
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>fSgDQ134</t>
-  </si>
-  <si>
-    <t>rkowlyw64</t>
-  </si>
-  <si>
-    <t>dMvH$2&amp;6</t>
+    <t>KZtcy695</t>
+  </si>
+  <si>
+    <t>bdcgwbt47</t>
+  </si>
+  <si>
+    <t>hJk7!3#R</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>DAeTNpEK</t>
-  </si>
-  <si>
-    <t>Rmvc</t>
+    <t>jjcBWIZR</t>
+  </si>
+  <si>
+    <t>hukc</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23081404</v>
+        <v>23081625</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding changes to P2,P3 of IExam
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>KZtcy695</t>
-  </si>
-  <si>
-    <t>bdcgwbt47</t>
-  </si>
-  <si>
-    <t>hJk7!3#R</t>
+    <t>qlksJ932</t>
+  </si>
+  <si>
+    <t>grxajwi65</t>
+  </si>
+  <si>
+    <t>c32!&amp;JrX</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>jjcBWIZR</t>
-  </si>
-  <si>
-    <t>hukc</t>
+    <t>TidmbvVd</t>
+  </si>
+  <si>
+    <t>frOZ</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23081625</v>
+        <v>23081808</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding p0 testcases for iAuthor
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>XwjNd171</t>
-  </si>
-  <si>
-    <t>usbmybz49</t>
-  </si>
-  <si>
-    <t>vTd2$D#6</t>
+    <t>Japhd932</t>
+  </si>
+  <si>
+    <t>gihbmrn38</t>
+  </si>
+  <si>
+    <t>pMD&amp;#32j</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>gBzTfrvq</t>
-  </si>
-  <si>
-    <t>Gcvw</t>
+    <t>RymAsYwy</t>
+  </si>
+  <si>
+    <t>jEHF</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23081822</v>
+        <v>23082104</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding Testcase and making few changes
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Japhd932</t>
-  </si>
-  <si>
-    <t>gihbmrn38</t>
-  </si>
-  <si>
-    <t>pMD&amp;#32j</t>
+    <t>XtGmt288</t>
+  </si>
+  <si>
+    <t>lrdubcp55</t>
+  </si>
+  <si>
+    <t>W%!Ew7p6</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>RymAsYwy</t>
-  </si>
-  <si>
-    <t>jEHF</t>
+    <t>QRsXPmJH</t>
+  </si>
+  <si>
+    <t>LOuB</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23082104</v>
+        <v>23082311</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added Reg iAuthor TC's
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Japhd932</t>
-  </si>
-  <si>
-    <t>gihbmrn38</t>
-  </si>
-  <si>
-    <t>pMD&amp;#32j</t>
+    <t>hokxh990</t>
+  </si>
+  <si>
+    <t>ydwykmq29</t>
+  </si>
+  <si>
+    <t>f&amp;vKG87$</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>RymAsYwy</t>
-  </si>
-  <si>
-    <t>jEHF</t>
+    <t>jVGZQLqQ</t>
+  </si>
+  <si>
+    <t>jWfj</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23082104</v>
+        <v>23082340</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding changes to Regression TC's
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>XtGmt288</t>
-  </si>
-  <si>
-    <t>lrdubcp55</t>
-  </si>
-  <si>
-    <t>W%!Ew7p6</t>
+    <t>hISZs664</t>
+  </si>
+  <si>
+    <t>gswjxye50</t>
+  </si>
+  <si>
+    <t>v%6Xx3F#</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>QRsXPmJH</t>
-  </si>
-  <si>
-    <t>LOuB</t>
+    <t>dVhilrjt</t>
+  </si>
+  <si>
+    <t>TeFY</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23082311</v>
+        <v>23082422</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding new testcases of iAuthor
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>hISZs664</t>
-  </si>
-  <si>
-    <t>gswjxye50</t>
-  </si>
-  <si>
-    <t>v%6Xx3F#</t>
+    <t>ZQnbB960</t>
+  </si>
+  <si>
+    <t>jdysrdy26</t>
+  </si>
+  <si>
+    <t>uWXd!&amp;97</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>dVhilrjt</t>
-  </si>
-  <si>
-    <t>TeFY</t>
+    <t>zSCmgXCC</t>
+  </si>
+  <si>
+    <t>rofG</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23082422</v>
+        <v>23083020</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding new testcases of iAuthor and iExam
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>xnVmb914</t>
-  </si>
-  <si>
-    <t>mwuqrpx90</t>
-  </si>
-  <si>
-    <t>BxY7e2#&amp;</t>
+    <t>PEKeK595</t>
+  </si>
+  <si>
+    <t>wrjxavd33</t>
+  </si>
+  <si>
+    <t>PmbY$5!7</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>VTlXAAGy</t>
-  </si>
-  <si>
-    <t>KMij</t>
+    <t>lmFrXCvp</t>
+  </si>
+  <si>
+    <t>Kssc</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23090109</v>
+        <v>23090411</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
added two cases and changed the smoke suite test case numbering
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>PEKeK595</t>
-  </si>
-  <si>
-    <t>wrjxavd33</t>
-  </si>
-  <si>
-    <t>PmbY$5!7</t>
+    <t>OBHCz204</t>
+  </si>
+  <si>
+    <t>vlgxpgw72</t>
+  </si>
+  <si>
+    <t>m6V!n5N#</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>lmFrXCvp</t>
-  </si>
-  <si>
-    <t>Kssc</t>
+    <t>EigazUKb</t>
+  </si>
+  <si>
+    <t>ReAG</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23090411</v>
+        <v>23090528</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding new testcases and adding qa and sandbox env
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>PEKeK595</t>
-  </si>
-  <si>
-    <t>wrjxavd33</t>
-  </si>
-  <si>
-    <t>PmbY$5!7</t>
+    <t>EUQFO344</t>
+  </si>
+  <si>
+    <t>qdpovyr35</t>
+  </si>
+  <si>
+    <t>RSyk6!&amp;5</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>lmFrXCvp</t>
-  </si>
-  <si>
-    <t>Kssc</t>
+    <t>UufeGBBt</t>
+  </si>
+  <si>
+    <t>QoYu</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23090411</v>
+        <v>23090529</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
added few cases and also added two new exams
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>OBHCz204</t>
-  </si>
-  <si>
-    <t>vlgxpgw72</t>
-  </si>
-  <si>
-    <t>m6V!n5N#</t>
+    <t>ZNbVv125</t>
+  </si>
+  <si>
+    <t>atucvvd74</t>
+  </si>
+  <si>
+    <t>u4#QqU!7</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>EigazUKb</t>
-  </si>
-  <si>
-    <t>ReAG</t>
+    <t>yMQASdYk</t>
+  </si>
+  <si>
+    <t>TwYw</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23090528</v>
+        <v>23090735</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding testcases fro iExam
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>OBHCz204</t>
-  </si>
-  <si>
-    <t>vlgxpgw72</t>
-  </si>
-  <si>
-    <t>m6V!n5N#</t>
+    <t>DzdbM298</t>
+  </si>
+  <si>
+    <t>xpxaoha41</t>
+  </si>
+  <si>
+    <t>y4N$&amp;u2W</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>EigazUKb</t>
-  </si>
-  <si>
-    <t>ReAG</t>
+    <t>hDXuMhdi</t>
+  </si>
+  <si>
+    <t>iDQt</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23090528</v>
+        <v>23090730</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added Reg iExam new TC's
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>SvKuk918</t>
-  </si>
-  <si>
-    <t>gucxmgd29</t>
-  </si>
-  <si>
-    <t>Xn5dN!%4</t>
+    <t>tQfkE733</t>
+  </si>
+  <si>
+    <t>dpjlgeo41</t>
+  </si>
+  <si>
+    <t>cp!5$H7A</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>jGNZdzNS</t>
-  </si>
-  <si>
-    <t>ZApI</t>
+    <t>PWrcmZOI</t>
+  </si>
+  <si>
+    <t>DMAu</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23090816</v>
+        <v>23091138</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
added couple of cases
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>SvKuk918</t>
-  </si>
-  <si>
-    <t>gucxmgd29</t>
-  </si>
-  <si>
-    <t>Xn5dN!%4</t>
+    <t>DFbVx581</t>
+  </si>
+  <si>
+    <t>dzhujzq74</t>
+  </si>
+  <si>
+    <t>Yk9&amp;4jZ#</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>jGNZdzNS</t>
-  </si>
-  <si>
-    <t>ZApI</t>
+    <t>YGScBgJI</t>
+  </si>
+  <si>
+    <t>TJVJ</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23090816</v>
+        <v>23091209</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding testcases of iExam
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>SvKuk918</t>
-  </si>
-  <si>
-    <t>gucxmgd29</t>
-  </si>
-  <si>
-    <t>Xn5dN!%4</t>
+    <t>DFbVx581</t>
+  </si>
+  <si>
+    <t>dzhujzq74</t>
+  </si>
+  <si>
+    <t>Yk9&amp;4jZ#</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>jGNZdzNS</t>
-  </si>
-  <si>
-    <t>ZApI</t>
+    <t>YGScBgJI</t>
+  </si>
+  <si>
+    <t>TJVJ</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23090816</v>
+        <v>23091209</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding testcases of iExam cases
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>DFbVx581</t>
-  </si>
-  <si>
-    <t>dzhujzq74</t>
-  </si>
-  <si>
-    <t>Yk9&amp;4jZ#</t>
+    <t>hsBJT120</t>
+  </si>
+  <si>
+    <t>rcuznfs75</t>
+  </si>
+  <si>
+    <t>Qp4T&amp;!n9</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>YGScBgJI</t>
-  </si>
-  <si>
-    <t>TJVJ</t>
+    <t>kJCJKswv</t>
+  </si>
+  <si>
+    <t>inor</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23091209</v>
+        <v>23091323</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
scripted couple of casses related to iEaxm
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>DFbVx581</t>
-  </si>
-  <si>
-    <t>dzhujzq74</t>
-  </si>
-  <si>
-    <t>Yk9&amp;4jZ#</t>
+    <t>myMvc790</t>
+  </si>
+  <si>
+    <t>rijbqfl34</t>
+  </si>
+  <si>
+    <t>S8n$g2P&amp;</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>YGScBgJI</t>
-  </si>
-  <si>
-    <t>TJVJ</t>
+    <t>LFTclhtR</t>
+  </si>
+  <si>
+    <t>kNDg</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23091209</v>
+        <v>23091356</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
adding updated TC for iExams
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>tCkfV986</t>
-  </si>
-  <si>
-    <t>sjfmbpc53</t>
-  </si>
-  <si>
-    <t>Jk#5T%8h</t>
+    <t>pPKtD203</t>
+  </si>
+  <si>
+    <t>rzljdex30</t>
+  </si>
+  <si>
+    <t>Wt&amp;5v2!B</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>uCWxYulc</t>
-  </si>
-  <si>
-    <t>qsZd</t>
+    <t>GznnOyiH</t>
+  </si>
+  <si>
+    <t>wGTi</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23091346</v>
+        <v>23091447</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added Reg modified P0 and P1 TC's
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>xLHlk358</t>
-  </si>
-  <si>
-    <t>chqahhv29</t>
-  </si>
-  <si>
-    <t>aG7M#2!t</t>
+    <t>ZmsjB128</t>
+  </si>
+  <si>
+    <t>ghqgnjf40</t>
+  </si>
+  <si>
+    <t>d2t8TK#!</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>LuvzfEwp</t>
-  </si>
-  <si>
-    <t>FudG</t>
+    <t>JrmqPOzF</t>
+  </si>
+  <si>
+    <t>aDfP</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23091444</v>
+        <v>23091535</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added Reg iProctor new TC's
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Paaiy259</t>
-  </si>
-  <si>
-    <t>qvmifem19</t>
-  </si>
-  <si>
-    <t>Qy9k2B$%</t>
+    <t>zspfU475</t>
+  </si>
+  <si>
+    <t>lovqcar73</t>
+  </si>
+  <si>
+    <t>B5%hKz&amp;4</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>lICnwatu</t>
-  </si>
-  <si>
-    <t>BEos</t>
+    <t>ZjFXctdn</t>
+  </si>
+  <si>
+    <t>eXgH</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23091477</v>
+        <v>23092023</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Modified Reg iProctor TC's
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>zspfU475</t>
-  </si>
-  <si>
-    <t>lovqcar73</t>
-  </si>
-  <si>
-    <t>B5%hKz&amp;4</t>
+    <t>cqBFJ752</t>
+  </si>
+  <si>
+    <t>amqfbph25</t>
+  </si>
+  <si>
+    <t>b32C%Kx#</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>ZjFXctdn</t>
-  </si>
-  <si>
-    <t>eXgH</t>
+    <t>JiMTvgut</t>
+  </si>
+  <si>
+    <t>YDAH</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23092023</v>
+        <v>23092132</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding iProctor testcases and modifying the cases
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>zspfU475</t>
-  </si>
-  <si>
-    <t>lovqcar73</t>
-  </si>
-  <si>
-    <t>B5%hKz&amp;4</t>
+    <t>LhfLJ648</t>
+  </si>
+  <si>
+    <t>wrqraym19</t>
+  </si>
+  <si>
+    <t>hQ!2$kJ3</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>ZjFXctdn</t>
-  </si>
-  <si>
-    <t>eXgH</t>
+    <t>TIktJnBp</t>
+  </si>
+  <si>
+    <t>hiZP</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23092023</v>
+        <v>23092133</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
optimising the code for iProctor cases
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>NLHAe773</t>
-  </si>
-  <si>
-    <t>kqjahxd94</t>
-  </si>
-  <si>
-    <t>S!sw3V&amp;2</t>
+    <t>JRmMF167</t>
+  </si>
+  <si>
+    <t>pcntnug55</t>
+  </si>
+  <si>
+    <t>t&amp;RM9!x6</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>utJBzSow</t>
-  </si>
-  <si>
-    <t>cggC</t>
+    <t>zdJMQuUb</t>
+  </si>
+  <si>
+    <t>fOTL</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23092282</v>
+        <v>23092933</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Modified Reg iExam TC's
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>NLHAe773</t>
-  </si>
-  <si>
-    <t>kqjahxd94</t>
-  </si>
-  <si>
-    <t>S!sw3V&amp;2</t>
+    <t>JRmMF167</t>
+  </si>
+  <si>
+    <t>pcntnug55</t>
+  </si>
+  <si>
+    <t>t&amp;RM9!x6</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>utJBzSow</t>
-  </si>
-  <si>
-    <t>cggC</t>
+    <t>zdJMQuUb</t>
+  </si>
+  <si>
+    <t>fOTL</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23092282</v>
+        <v>23092933</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
adding changes to iproctor and adding new testcases to iAuthor
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>JRmMF167</t>
-  </si>
-  <si>
-    <t>pcntnug55</t>
-  </si>
-  <si>
-    <t>t&amp;RM9!x6</t>
+    <t>LlpiO680</t>
+  </si>
+  <si>
+    <t>pfrfhqs65</t>
+  </si>
+  <si>
+    <t>x3%Q!zK6</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>zdJMQuUb</t>
-  </si>
-  <si>
-    <t>fOTL</t>
+    <t>GQQiMXYY</t>
+  </si>
+  <si>
+    <t>lJVC</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23092933</v>
+        <v>231004243</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding new testcases for iAuthor and changing smoke suite of iProctor
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="users" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>nOAqy342</t>
-  </si>
-  <si>
-    <t>ncgappg66</t>
-  </si>
-  <si>
-    <t>Q%!f6gW5</t>
+    <t>ZhyoF284</t>
+  </si>
+  <si>
+    <t>qfzzgjw49</t>
+  </si>
+  <si>
+    <t>A&amp;3sP!h6</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>ngOyQKMX</t>
-  </si>
-  <si>
-    <t>BjWC</t>
+    <t>xgWJZTBa</t>
+  </si>
+  <si>
+    <t>ydGc</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -67,18 +67,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -98,34 +89,14 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -430,60 +401,60 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:H2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2">
-        <v>231004239</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2">
+        <v>23100602</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new testcases for iAuthor
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>ZhyoF284</t>
-  </si>
-  <si>
-    <t>qfzzgjw49</t>
-  </si>
-  <si>
-    <t>A&amp;3sP!h6</t>
+    <t>DinEb858</t>
+  </si>
+  <si>
+    <t>mspthlv47</t>
+  </si>
+  <si>
+    <t>TBa73y#$</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>xgWJZTBa</t>
-  </si>
-  <si>
-    <t>ydGc</t>
+    <t>PNpMBuFk</t>
+  </si>
+  <si>
+    <t>mMDY</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23100602</v>
+        <v>231009312</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding new iAuthor testcases
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>ZhyoF284</t>
-  </si>
-  <si>
-    <t>qfzzgjw49</t>
-  </si>
-  <si>
-    <t>A&amp;3sP!h6</t>
+    <t>FkJUh993</t>
+  </si>
+  <si>
+    <t>qhonvob32</t>
+  </si>
+  <si>
+    <t>n%aN5&amp;G8</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>xgWJZTBa</t>
-  </si>
-  <si>
-    <t>ydGc</t>
+    <t>kDjuRTMy</t>
+  </si>
+  <si>
+    <t>Qfuf</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23100602</v>
+        <v>231010291</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding new iProctor smoke testcases changes
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>PnucB683</t>
-  </si>
-  <si>
-    <t>iagevts83</t>
-  </si>
-  <si>
-    <t>k#9F!U5p</t>
+    <t>jMtSL985</t>
+  </si>
+  <si>
+    <t>ipwxppd82</t>
+  </si>
+  <si>
+    <t>kR82P&amp;%u</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>JsKDMsBN</t>
-  </si>
-  <si>
-    <t>tFYn</t>
+    <t>OMCJfClL</t>
+  </si>
+  <si>
+    <t>CELt</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23110202</v>
+        <v>23110301</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Adding changes in iAuthor
</commit_message>
<xml_diff>
--- a/download/User_details.xlsx
+++ b/download/User_details.xlsx
@@ -41,22 +41,22 @@
     <t>Role</t>
   </si>
   <si>
-    <t>fyOYs108</t>
-  </si>
-  <si>
-    <t>xvifvfo50</t>
-  </si>
-  <si>
-    <t>hEM8#9t&amp;</t>
+    <t>iRiaL673</t>
+  </si>
+  <si>
+    <t>zwqhjhs73</t>
+  </si>
+  <si>
+    <t>sv9XR7$#</t>
   </si>
   <si>
     <t>MR</t>
   </si>
   <si>
-    <t>POfOYRdX</t>
-  </si>
-  <si>
-    <t>zdJO</t>
+    <t>psabtdSX</t>
+  </si>
+  <si>
+    <t>TVAM</t>
   </si>
   <si>
     <t>Candidate</t>
@@ -437,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>23110716</v>
+        <v>23110860</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>